<commit_message>
大改未成形 添加UITextrue 4-29 20
</commit_message>
<xml_diff>
--- a/Assets/Resources/Form/Item.xlsx
+++ b/Assets/Resources/Form/Item.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAB0731-5712-432F-A857-CAC3397871B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB393521-7EF7-4CCF-85BD-26207E7869EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,10 +26,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>刀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>棒</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -68,6 +64,9 @@
   <si>
     <t>攻击速度</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Knife</t>
   </si>
 </sst>
 </file>
@@ -395,29 +394,29 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -425,10 +424,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -445,10 +444,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -465,10 +464,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>30</v>

</xml_diff>